<commit_message>
translations reworked for dino integration
</commit_message>
<xml_diff>
--- a/formats/testdata/languages.xlsx
+++ b/formats/testdata/languages.xlsx
@@ -32,10 +32,10 @@
     <t xml:space="preserve">label</t>
   </si>
   <si>
-    <t xml:space="preserve">label::German (de)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">label::Italian (it)</t>
+    <t xml:space="preserve">label::DEU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label::ITA</t>
   </si>
   <si>
     <t xml:space="preserve">begin group</t>
@@ -216,23 +216,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -321,8 +320,8 @@
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -331,23 +330,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -420,8 +418,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>